<commit_message>
- Add to local branch
</commit_message>
<xml_diff>
--- a/document/report accounting/FORM BANG KE  NHA THAU.xlsx
+++ b/document/report accounting/FORM BANG KE  NHA THAU.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Working\Projects\GitHub\ael\document\report accounting\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -21,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>BẢNG KÊ VẬN CHUYỂN</t>
   </si>
@@ -115,6 +110,21 @@
   </si>
   <si>
     <t>Khác</t>
+  </si>
+  <si>
+    <t>Nhà thầu</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Phí hQ</t>
   </si>
 </sst>
 </file>
@@ -125,7 +135,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,8 +207,15 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,6 +231,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -298,7 +321,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -320,9 +343,6 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -347,13 +367,25 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="23" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="45">
     <cellStyle name="Comma 2 10" xfId="2"/>
@@ -458,7 +490,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -493,7 +525,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -702,10 +734,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U29"/>
+  <dimension ref="A1:V29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,58 +750,68 @@
     <col min="13" max="13" width="10.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="19.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:22" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-    </row>
-    <row r="2" spans="1:21" ht="19.5" x14ac:dyDescent="0.3">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
+      <c r="R1" s="20"/>
+      <c r="S1" s="20"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+    </row>
+    <row r="2" spans="1:22" ht="19.5" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
+      <c r="D2" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>32</v>
+      </c>
       <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="J2" s="2"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="13"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
+      <c r="P2" s="17"/>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
-      <c r="S2" s="1"/>
+      <c r="S2" s="2"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
-    </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V2" s="1"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="18" t="s">
         <v>28</v>
       </c>
       <c r="D3" s="1"/>
@@ -787,19 +829,20 @@
       <c r="N3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="1"/>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19"/>
+      <c r="Q3" s="19"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="19"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
-    </row>
-    <row r="4" spans="1:21" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V3" s="1"/>
+    </row>
+    <row r="4" spans="1:22" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
@@ -832,35 +875,38 @@
       <c r="L4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="M4" s="17" t="s">
+      <c r="M4" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="9" t="s">
+      <c r="N4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="13" t="s">
+      <c r="O4" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="9" t="s">
+      <c r="P4" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q4" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" s="10" t="s">
+      <c r="R4" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="R4" s="10" t="s">
+      <c r="S4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="12" t="s">
+      <c r="T4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="T4" s="12" t="s">
+      <c r="U4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="U4" s="11" t="s">
+      <c r="V4" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>1</v>
       </c>
@@ -884,8 +930,9 @@
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
       <c r="U5" s="3"/>
-    </row>
-    <row r="6" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V5" s="3"/>
+    </row>
+    <row r="6" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>2</v>
       </c>
@@ -909,8 +956,9 @@
       <c r="S6" s="3"/>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
-    </row>
-    <row r="7" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V6" s="3"/>
+    </row>
+    <row r="7" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>3</v>
       </c>
@@ -934,8 +982,9 @@
       <c r="S7" s="3"/>
       <c r="T7" s="3"/>
       <c r="U7" s="3"/>
-    </row>
-    <row r="8" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V7" s="3"/>
+    </row>
+    <row r="8" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>4</v>
       </c>
@@ -959,8 +1008,9 @@
       <c r="S8" s="3"/>
       <c r="T8" s="3"/>
       <c r="U8" s="3"/>
-    </row>
-    <row r="9" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V8" s="3"/>
+    </row>
+    <row r="9" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>5</v>
       </c>
@@ -984,8 +1034,9 @@
       <c r="S9" s="3"/>
       <c r="T9" s="3"/>
       <c r="U9" s="3"/>
-    </row>
-    <row r="10" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V9" s="3"/>
+    </row>
+    <row r="10" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>6</v>
       </c>
@@ -1009,8 +1060,9 @@
       <c r="S10" s="3"/>
       <c r="T10" s="3"/>
       <c r="U10" s="3"/>
-    </row>
-    <row r="11" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V10" s="3"/>
+    </row>
+    <row r="11" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>7</v>
       </c>
@@ -1034,8 +1086,9 @@
       <c r="S11" s="3"/>
       <c r="T11" s="3"/>
       <c r="U11" s="3"/>
-    </row>
-    <row r="12" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V11" s="3"/>
+    </row>
+    <row r="12" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -1059,8 +1112,9 @@
       <c r="S12" s="3"/>
       <c r="T12" s="3"/>
       <c r="U12" s="3"/>
-    </row>
-    <row r="13" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V12" s="3"/>
+    </row>
+    <row r="13" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -1084,8 +1138,9 @@
       <c r="S13" s="3"/>
       <c r="T13" s="3"/>
       <c r="U13" s="3"/>
-    </row>
-    <row r="14" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V13" s="3"/>
+    </row>
+    <row r="14" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -1109,8 +1164,9 @@
       <c r="S14" s="3"/>
       <c r="T14" s="3"/>
       <c r="U14" s="3"/>
-    </row>
-    <row r="15" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V14" s="3"/>
+    </row>
+    <row r="15" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>11</v>
       </c>
@@ -1134,8 +1190,9 @@
       <c r="S15" s="3"/>
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
-    </row>
-    <row r="16" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V15" s="3"/>
+    </row>
+    <row r="16" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>12</v>
       </c>
@@ -1159,8 +1216,9 @@
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
       <c r="U16" s="3"/>
-    </row>
-    <row r="17" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V16" s="3"/>
+    </row>
+    <row r="17" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>13</v>
       </c>
@@ -1184,8 +1242,9 @@
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
       <c r="U17" s="3"/>
-    </row>
-    <row r="18" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V17" s="3"/>
+    </row>
+    <row r="18" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>14</v>
       </c>
@@ -1209,8 +1268,9 @@
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
       <c r="U18" s="3"/>
-    </row>
-    <row r="19" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V18" s="3"/>
+    </row>
+    <row r="19" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>15</v>
       </c>
@@ -1234,8 +1294,9 @@
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
       <c r="U19" s="3"/>
-    </row>
-    <row r="20" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V19" s="3"/>
+    </row>
+    <row r="20" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>16</v>
       </c>
@@ -1259,8 +1320,9 @@
       <c r="S20" s="3"/>
       <c r="T20" s="3"/>
       <c r="U20" s="3"/>
-    </row>
-    <row r="21" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V20" s="3"/>
+    </row>
+    <row r="21" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>17</v>
       </c>
@@ -1284,8 +1346,9 @@
       <c r="S21" s="3"/>
       <c r="T21" s="3"/>
       <c r="U21" s="3"/>
-    </row>
-    <row r="22" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="V21" s="3"/>
+    </row>
+    <row r="22" spans="1:22" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>18</v>
       </c>
@@ -1309,8 +1372,9 @@
       <c r="S22" s="3"/>
       <c r="T22" s="3"/>
       <c r="U22" s="3"/>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V22" s="3"/>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>23</v>
       </c>
@@ -1318,7 +1382,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>25</v>
       </c>
@@ -1331,8 +1395,8 @@
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="O3:R3"/>
-    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="O3:S3"/>
+    <mergeCell ref="A1:V1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>